<commit_message>
incremento de verificação das jogadas
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,26 +450,78 @@
       <c r="C1" t="n">
         <v>0</v>
       </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalização da aba de configuração
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="jogo1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="configurações" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="jogo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,6 +433,61 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Linhas</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Colunas</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dificuldade</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -445,16 +501,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
         <v>-1</v>
-      </c>
-      <c r="C1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -465,27 +521,27 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
         <v>-1</v>
       </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
       <c r="D3" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -496,13 +552,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>-1</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -516,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
correção no modulo de geração de bombas
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -449,7 +449,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -488,7 +488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,28 +506,16 @@
       <c r="C1" t="n">
         <v>0</v>
       </c>
-      <c r="D1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" t="n">
-        <v>-1</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -539,46 +527,6 @@
       </c>
       <c r="C3" t="n">
         <v>-1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção da contagem de bombas ao redor
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -48,11 +47,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -131,10 +136,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -172,69 +177,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -258,54 +265,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -315,7 +321,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -324,7 +330,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -333,7 +339,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -341,10 +347,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -373,7 +379,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -386,13 +392,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -412,7 +417,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A1"/>
@@ -423,14 +428,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B3"/>
@@ -440,96 +445,181 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Linhas</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Colunas</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Dificuldade</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" t="n">
-        <v>0</v>
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-1</v>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CORREÇÃO DO BUG QUANDO O NUMERO É MAIOR QUUE O TABULEIRO
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="configurações" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="jogo" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="configurações" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="jogo" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,14 +414,45 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Linhas</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Colunas</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dificuldade</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -433,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,184 +474,51 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Linhas</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>5</v>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Colunas</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5</v>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dificuldade</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>